<commit_message>
Add key event about new COO in £BIDS
</commit_message>
<xml_diff>
--- a/£BIDS.xlsx
+++ b/£BIDS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23818A1-46D3-4B1B-B309-2D282C5ABBBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9994D2C-A4F4-4235-A612-A7F748150338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="18900" xr2:uid="{DFFD8AD2-463C-4EE9-AB45-D04A4DE50CB4}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="118">
   <si>
     <t>£BIDS</t>
   </si>
@@ -124,12 +124,6 @@
     <t>CFO</t>
   </si>
   <si>
-    <t>CTO?</t>
-  </si>
-  <si>
-    <t>Chairman</t>
-  </si>
-  <si>
     <t>Publishers &amp; Games using Bidstack Tech</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>Hyperscape</t>
   </si>
   <si>
-    <t>Train Sim World 2</t>
-  </si>
-  <si>
     <t>Advertising Using Bidstack Tech</t>
   </si>
   <si>
@@ -340,9 +331,6 @@
     <t>London, UK</t>
   </si>
   <si>
-    <t>2016?</t>
-  </si>
-  <si>
     <t>Kellogg's (Pringles)</t>
   </si>
   <si>
@@ -353,6 +341,45 @@
   </si>
   <si>
     <t>Strategic investor provides £5m in investment along with another £5m placing @ 2.85</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>Camila Franklin</t>
+  </si>
+  <si>
+    <t>Tesco</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>L'Oreal</t>
+  </si>
+  <si>
+    <t>Playmobil</t>
+  </si>
+  <si>
+    <t>Redbull</t>
+  </si>
+  <si>
+    <t>Current COO, Lisa Hau now working as Chief Strategy Officer &amp; remains on board</t>
+  </si>
+  <si>
+    <t>Bidstack appoint former AdColony COO Camila Franklin as £BIDS COO</t>
+  </si>
+  <si>
+    <t>CSO</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Lisa Hau</t>
+  </si>
+  <si>
+    <t>Train Sim World 2/3</t>
   </si>
 </sst>
 </file>
@@ -366,7 +393,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +469,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Araial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -576,7 +610,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -647,7 +681,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -695,9 +728,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -707,15 +755,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -728,7 +767,15 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -757,13 +804,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>127289</xdr:rowOff>
+      <xdr:rowOff>146339</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -793,7 +840,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2714625" y="57150"/>
+          <a:off x="2714625" y="76200"/>
           <a:ext cx="571500" cy="584489"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1221,7 +1268,7 @@
   <dimension ref="B2:AA43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1240,49 +1287,45 @@
       </c>
     </row>
     <row r="5" spans="2:27">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="80"/>
-      <c r="H5" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="80"/>
-      <c r="S5" s="78" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="79"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="80"/>
-      <c r="X5" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y5" s="79"/>
-      <c r="Z5" s="79"/>
-      <c r="AA5" s="80"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="77"/>
+      <c r="H5" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="77"/>
+      <c r="S5" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="77"/>
+      <c r="X5" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="76"/>
+      <c r="AA5" s="77"/>
     </row>
     <row r="6" spans="2:27">
       <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="34">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D6" s="57"/>
-      <c r="H6" s="35">
-        <v>44835</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>108</v>
-      </c>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D6" s="56"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="36"/>
       <c r="K6" s="36"/>
       <c r="L6" s="36"/>
@@ -1290,14 +1333,14 @@
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="37"/>
-      <c r="S6" s="85" t="s">
-        <v>47</v>
+      <c r="S6" s="78" t="s">
+        <v>44</v>
       </c>
       <c r="T6" s="73"/>
       <c r="U6" s="73"/>
       <c r="V6" s="74"/>
       <c r="X6" s="38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Y6" s="36"/>
       <c r="Z6" s="36"/>
@@ -1310,8 +1353,8 @@
       <c r="C7" s="39">
         <v>932.53</v>
       </c>
-      <c r="D7" s="57" t="s">
-        <v>9</v>
+      <c r="D7" s="56" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="40"/>
       <c r="I7" s="36"/>
@@ -1322,14 +1365,14 @@
       <c r="N7" s="36"/>
       <c r="O7" s="36"/>
       <c r="P7" s="37"/>
-      <c r="S7" s="85" t="s">
-        <v>48</v>
+      <c r="S7" s="78" t="s">
+        <v>45</v>
       </c>
       <c r="T7" s="73"/>
       <c r="U7" s="73"/>
       <c r="V7" s="74"/>
       <c r="X7" s="41" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="Y7" s="36"/>
       <c r="Z7" s="36"/>
@@ -1341,9 +1384,9 @@
       </c>
       <c r="C8" s="42">
         <f>C6*C7</f>
-        <v>31.706020000000002</v>
-      </c>
-      <c r="D8" s="57"/>
+        <v>26.11084</v>
+      </c>
+      <c r="D8" s="56"/>
       <c r="H8" s="40"/>
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
@@ -1353,8 +1396,8 @@
       <c r="N8" s="36"/>
       <c r="O8" s="36"/>
       <c r="P8" s="37"/>
-      <c r="S8" s="85" t="s">
-        <v>49</v>
+      <c r="S8" s="78" t="s">
+        <v>46</v>
       </c>
       <c r="T8" s="73"/>
       <c r="U8" s="73"/>
@@ -1371,11 +1414,15 @@
       <c r="C9" s="39">
         <v>3.7</v>
       </c>
-      <c r="D9" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="36"/>
+      <c r="D9" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="35">
+        <v>44835</v>
+      </c>
+      <c r="I9" s="86" t="s">
+        <v>113</v>
+      </c>
       <c r="J9" s="36"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
@@ -1383,14 +1430,14 @@
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
       <c r="P9" s="37"/>
-      <c r="S9" s="85" t="s">
-        <v>50</v>
+      <c r="S9" s="78" t="s">
+        <v>47</v>
       </c>
       <c r="T9" s="73"/>
       <c r="U9" s="73"/>
       <c r="V9" s="74"/>
       <c r="X9" s="38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
@@ -1403,14 +1450,12 @@
       <c r="C10" s="39">
         <v>0</v>
       </c>
-      <c r="D10" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="35">
-        <v>44743</v>
-      </c>
-      <c r="I10" s="36" t="s">
-        <v>80</v>
+      <c r="D10" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="87" t="s">
+        <v>112</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="36"/>
@@ -1419,14 +1464,14 @@
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
       <c r="P10" s="37"/>
-      <c r="S10" s="85" t="s">
-        <v>105</v>
+      <c r="S10" s="78" t="s">
+        <v>101</v>
       </c>
       <c r="T10" s="73"/>
       <c r="U10" s="73"/>
       <c r="V10" s="74"/>
       <c r="X10" s="41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="36"/>
       <c r="Z10" s="36"/>
@@ -1440,13 +1485,11 @@
         <f>C9-C10</f>
         <v>3.7</v>
       </c>
-      <c r="D11" s="57" t="s">
-        <v>9</v>
+      <c r="D11" s="56" t="s">
+        <v>19</v>
       </c>
       <c r="H11" s="40"/>
-      <c r="I11" s="54" t="s">
-        <v>81</v>
-      </c>
+      <c r="I11" s="36"/>
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
@@ -1454,12 +1497,12 @@
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
       <c r="P11" s="37"/>
-      <c r="S11" s="77" t="s">
-        <v>51</v>
-      </c>
-      <c r="T11" s="75"/>
-      <c r="U11" s="75"/>
-      <c r="V11" s="76"/>
+      <c r="S11" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="T11" s="73"/>
+      <c r="U11" s="73"/>
+      <c r="V11" s="74"/>
       <c r="X11" s="38"/>
       <c r="Y11" s="36"/>
       <c r="Z11" s="36"/>
@@ -1471,9 +1514,9 @@
       </c>
       <c r="C12" s="45">
         <f>C8-C11</f>
-        <v>28.006020000000003</v>
-      </c>
-      <c r="D12" s="58"/>
+        <v>22.41084</v>
+      </c>
+      <c r="D12" s="57"/>
       <c r="H12" s="40"/>
       <c r="I12" s="36"/>
       <c r="J12" s="36"/>
@@ -1483,8 +1526,14 @@
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
       <c r="P12" s="37"/>
+      <c r="S12" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="T12" s="73"/>
+      <c r="U12" s="73"/>
+      <c r="V12" s="74"/>
       <c r="X12" s="38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y12" s="36"/>
       <c r="Z12" s="36"/>
@@ -1494,8 +1543,12 @@
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="36"/>
+      <c r="H13" s="35">
+        <v>44835</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>104</v>
+      </c>
       <c r="J13" s="36"/>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
@@ -1503,8 +1556,14 @@
       <c r="N13" s="36"/>
       <c r="O13" s="36"/>
       <c r="P13" s="37"/>
+      <c r="S13" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="T13" s="73"/>
+      <c r="U13" s="73"/>
+      <c r="V13" s="74"/>
       <c r="X13" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Y13" s="36"/>
       <c r="Z13" s="36"/>
@@ -1523,19 +1582,25 @@
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
       <c r="P14" s="37"/>
+      <c r="S14" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="T14" s="73"/>
+      <c r="U14" s="73"/>
+      <c r="V14" s="74"/>
       <c r="X14" s="41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Y14" s="36"/>
       <c r="Z14" s="36"/>
       <c r="AA14" s="37"/>
     </row>
     <row r="15" spans="2:27">
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="80"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="77"/>
       <c r="H15" s="40"/>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
@@ -1545,17 +1610,23 @@
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
       <c r="P15" s="37"/>
+      <c r="S15" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="T15" s="73"/>
+      <c r="U15" s="73"/>
+      <c r="V15" s="74"/>
       <c r="X15" s="43"/>
       <c r="Y15" s="36"/>
       <c r="Z15" s="36"/>
       <c r="AA15" s="37"/>
     </row>
     <row r="16" spans="2:27">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="89" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D16" s="74"/>
       <c r="H16" s="40"/>
@@ -1567,21 +1638,31 @@
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
       <c r="P16" s="37"/>
+      <c r="S16" s="81" t="s">
+        <v>48</v>
+      </c>
+      <c r="T16" s="79"/>
+      <c r="U16" s="79"/>
+      <c r="V16" s="80"/>
       <c r="X16" s="38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Y16" s="36"/>
       <c r="Z16" s="36"/>
       <c r="AA16" s="37"/>
     </row>
     <row r="17" spans="2:27">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="89" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="73"/>
       <c r="D17" s="74"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="36"/>
+      <c r="H17" s="35">
+        <v>44743</v>
+      </c>
+      <c r="I17" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="J17" s="36"/>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
@@ -1590,20 +1671,24 @@
       <c r="O17" s="36"/>
       <c r="P17" s="37"/>
       <c r="X17" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Y17" s="36"/>
       <c r="Z17" s="36"/>
       <c r="AA17" s="37"/>
     </row>
     <row r="18" spans="2:27">
-      <c r="B18" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="73"/>
+      <c r="B18" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>106</v>
+      </c>
       <c r="D18" s="74"/>
       <c r="H18" s="40"/>
-      <c r="I18" s="36"/>
+      <c r="I18" s="53" t="s">
+        <v>78</v>
+      </c>
       <c r="J18" s="36"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
@@ -1617,9 +1702,13 @@
       <c r="AA18" s="37"/>
     </row>
     <row r="19" spans="2:27">
-      <c r="B19" s="43"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
+      <c r="B19" s="89" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="74"/>
       <c r="H19" s="40"/>
       <c r="I19" s="36"/>
       <c r="J19" s="36"/>
@@ -1630,20 +1719,20 @@
       <c r="O19" s="36"/>
       <c r="P19" s="37"/>
       <c r="X19" s="38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Y19" s="36"/>
       <c r="Z19" s="36"/>
       <c r="AA19" s="37"/>
     </row>
     <row r="20" spans="2:27">
-      <c r="B20" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="75" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="76"/>
+      <c r="B20" s="90" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="80"/>
       <c r="H20" s="40"/>
       <c r="I20" s="36"/>
       <c r="J20" s="36"/>
@@ -1684,18 +1773,18 @@
       <c r="O22" s="36"/>
       <c r="P22" s="37"/>
       <c r="X22" s="38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Y22" s="36"/>
       <c r="Z22" s="36"/>
       <c r="AA22" s="37"/>
     </row>
     <row r="23" spans="2:27">
-      <c r="B23" s="78" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="80"/>
+      <c r="B23" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="76"/>
+      <c r="D23" s="77"/>
       <c r="H23" s="40"/>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
@@ -1705,8 +1794,8 @@
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
       <c r="P23" s="37"/>
-      <c r="X23" s="49" t="s">
-        <v>40</v>
+      <c r="X23" s="48" t="s">
+        <v>38</v>
       </c>
       <c r="Y23" s="36"/>
       <c r="Z23" s="36"/>
@@ -1714,10 +1803,10 @@
     </row>
     <row r="24" spans="2:27">
       <c r="B24" s="40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="73" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D24" s="74"/>
       <c r="H24" s="40"/>
@@ -1729,8 +1818,8 @@
       <c r="N24" s="36"/>
       <c r="O24" s="36"/>
       <c r="P24" s="37"/>
-      <c r="X24" s="49" t="s">
-        <v>41</v>
+      <c r="X24" s="48" t="s">
+        <v>39</v>
       </c>
       <c r="Y24" s="36"/>
       <c r="Z24" s="36"/>
@@ -1738,10 +1827,10 @@
     </row>
     <row r="25" spans="2:27">
       <c r="B25" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>104</v>
+        <v>82</v>
+      </c>
+      <c r="C25" s="73">
+        <v>2016</v>
       </c>
       <c r="D25" s="74"/>
       <c r="H25" s="40"/>
@@ -1753,8 +1842,8 @@
       <c r="N25" s="36"/>
       <c r="O25" s="36"/>
       <c r="P25" s="37"/>
-      <c r="X25" s="49" t="s">
-        <v>42</v>
+      <c r="X25" s="48" t="s">
+        <v>40</v>
       </c>
       <c r="Y25" s="36"/>
       <c r="Z25" s="36"/>
@@ -1773,26 +1862,26 @@
       <c r="N26" s="36"/>
       <c r="O26" s="36"/>
       <c r="P26" s="37"/>
-      <c r="X26" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="52"/>
+      <c r="X26" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="51"/>
     </row>
     <row r="27" spans="2:27">
       <c r="B27" s="40"/>
       <c r="C27" s="46"/>
       <c r="D27" s="47"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="51"/>
     </row>
     <row r="28" spans="2:27">
       <c r="B28" s="40"/>
@@ -1806,72 +1895,72 @@
     </row>
     <row r="30" spans="2:27">
       <c r="B30" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="74"/>
+      <c r="D30" s="88"/>
     </row>
     <row r="31" spans="2:27">
-      <c r="B31" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="84"/>
+      <c r="B31" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="85"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="78" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="79"/>
-      <c r="D34" s="80"/>
+      <c r="B34" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="76"/>
+      <c r="D34" s="77"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="81">
+        <v>102</v>
+      </c>
+      <c r="C35" s="82">
         <f>C8/'Financial Model'!C14+'Financial Model'!C14</f>
-        <v>-12.948076476743388</v>
-      </c>
-      <c r="D35" s="82"/>
+        <v>-11.241799745553379</v>
+      </c>
+      <c r="D35" s="83"/>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60"/>
+        <v>93</v>
+      </c>
+      <c r="C36" s="58"/>
+      <c r="D36" s="59"/>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="73"/>
       <c r="D37" s="74"/>
       <c r="H37" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="40" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="74"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="81">
+        <v>96</v>
+      </c>
+      <c r="C39" s="82">
         <f>C6/'Financial Model'!F49</f>
-        <v>5.9887885347261767</v>
-      </c>
-      <c r="D39" s="82"/>
+        <v>4.9319434991862634</v>
+      </c>
+      <c r="D39" s="83"/>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="40"/>
@@ -1880,27 +1969,48 @@
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="40" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C41" s="73"/>
       <c r="D41" s="74"/>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C42" s="73"/>
       <c r="D42" s="74"/>
     </row>
     <row r="43" spans="2:8">
-      <c r="B43" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="76"/>
+      <c r="B43" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="79"/>
+      <c r="D43" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="37">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="S15:V15"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="S11:V11"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -1917,29 +2027,14 @@
     <mergeCell ref="S6:V6"/>
     <mergeCell ref="S7:V7"/>
     <mergeCell ref="S8:V8"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{E4B851AE-A6B7-0248-9880-6DBD666C28BA}"/>
+    <hyperlink ref="I9" r:id="rId2" display="Bidstack appoint Camila Franklin as COO" xr:uid="{91406AA9-3DB6-4F3F-9F60-8807BC447FC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1948,10 +2043,10 @@
   <dimension ref="A1:T59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J70" sqref="J70"/>
+      <selection pane="bottomRight" activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1986,7 +2081,7 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -2030,7 +2125,7 @@
         <v>44561</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -2058,7 +2153,7 @@
         <f>L3-D3</f>
         <v>1.8032770000000002</v>
       </c>
-      <c r="F3" s="61">
+      <c r="F3" s="60">
         <v>2.0459860000000001</v>
       </c>
       <c r="G3" s="12"/>
@@ -2095,7 +2190,7 @@
         <f>L4-D4</f>
         <v>1.136881</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="61">
         <v>1.229225</v>
       </c>
       <c r="G4" s="12"/>
@@ -2133,7 +2228,7 @@
         <f>E3-E4</f>
         <v>0.66639600000000021</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="60">
         <f>F3-F4</f>
         <v>0.81676100000000007</v>
       </c>
@@ -2159,7 +2254,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B6" s="14">
         <v>3.2448890000000001</v>
@@ -2175,7 +2270,7 @@
         <f>L6-D6</f>
         <v>4.7660529999999994</v>
       </c>
-      <c r="F6" s="61">
+      <c r="F6" s="60">
         <v>4.5075010000000004</v>
       </c>
       <c r="G6" s="12"/>
@@ -2198,7 +2293,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" s="14">
         <v>0</v>
@@ -2214,7 +2309,7 @@
         <f>L7-D7</f>
         <v>0.222555</v>
       </c>
-      <c r="F7" s="61">
+      <c r="F7" s="60">
         <v>0</v>
       </c>
       <c r="G7" s="12"/>
@@ -2235,7 +2330,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" s="14">
         <f>B7+B6</f>
@@ -2253,7 +2348,7 @@
         <f>E7+E6</f>
         <v>4.9886079999999993</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="61">
         <f>F7+F6</f>
         <v>4.5075010000000004</v>
       </c>
@@ -2280,7 +2375,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B9" s="10">
         <f>B5-B8</f>
@@ -2298,7 +2393,7 @@
         <f>E5-E8</f>
         <v>-4.3222119999999986</v>
       </c>
-      <c r="F9" s="61">
+      <c r="F9" s="60">
         <f>F5-F8</f>
         <v>-3.6907400000000004</v>
       </c>
@@ -2324,7 +2419,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B10" s="14">
         <v>2.3519999999999999E-3</v>
@@ -2340,7 +2435,7 @@
         <f>L10-D10</f>
         <v>1.2000000000000002E-4</v>
       </c>
-      <c r="F10" s="61">
+      <c r="F10" s="60">
         <v>9.6000000000000002E-4</v>
       </c>
       <c r="G10" s="18"/>
@@ -2361,7 +2456,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B11" s="14">
         <v>6.9999999999999999E-4</v>
@@ -2377,7 +2472,7 @@
         <f>L11-D11</f>
         <v>3.2320000000000001E-3</v>
       </c>
-      <c r="F11" s="61">
+      <c r="F11" s="60">
         <v>1.4419999999999999E-3</v>
       </c>
       <c r="G11" s="18"/>
@@ -2398,7 +2493,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="14">
         <f>B9+B10-B11</f>
@@ -2416,7 +2511,7 @@
         <f>E9+E10-E11</f>
         <v>-4.3253239999999984</v>
       </c>
-      <c r="F12" s="62">
+      <c r="F12" s="61">
         <f>F9+F10-F11</f>
         <v>-3.6912220000000002</v>
       </c>
@@ -2442,7 +2537,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" s="14">
         <v>-5.0493000000000003E-2</v>
@@ -2458,7 +2553,7 @@
         <f>L13-D13</f>
         <v>-0.91627100000000006</v>
       </c>
-      <c r="F13" s="62">
+      <c r="F13" s="61">
         <v>-0.93818400000000002</v>
       </c>
       <c r="G13" s="18"/>
@@ -2478,7 +2573,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="10">
         <f>B12-B13</f>
@@ -2496,7 +2591,7 @@
         <f>E12-E13</f>
         <v>-3.4090529999999983</v>
       </c>
-      <c r="F14" s="61">
+      <c r="F14" s="60">
         <f>F12-F13</f>
         <v>-2.7530380000000001</v>
       </c>
@@ -2520,7 +2615,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="20">
         <f>B14/B16</f>
@@ -2802,7 +2897,7 @@
         <f>C3/B3-1</f>
         <v>4.186610429839571</v>
       </c>
-      <c r="D25" s="56">
+      <c r="D25" s="55">
         <f>D3/C3-1</f>
         <v>-0.42306553240462286</v>
       </c>
@@ -2810,22 +2905,22 @@
         <f>E3/D3-1</f>
         <v>1.1987536213506056</v>
       </c>
-      <c r="F25" s="56">
+      <c r="F25" s="55">
         <f>F3/E3-1</f>
         <v>0.13459329875554338</v>
       </c>
       <c r="G25" s="23"/>
-      <c r="J25" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="K25" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="L25" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="M25" s="64" t="s">
-        <v>90</v>
+      <c r="J25" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="K25" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="L25" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -2835,9 +2930,9 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="66">
+        <v>63</v>
+      </c>
+      <c r="E29" s="65">
         <f>L29</f>
         <v>7.28E-3</v>
       </c>
@@ -2851,29 +2946,32 @@
         <v>7.28E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="2" t="s">
-        <v>67</v>
-      </c>
+    <row r="30" spans="1:13" s="6" customFormat="1">
+      <c r="A30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="26"/>
       <c r="E30" s="66">
         <f t="shared" ref="E30:E49" si="5">L30</f>
         <v>7.4778409999999997</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="31">
         <v>0</v>
       </c>
-      <c r="K30" s="30">
+      <c r="G30" s="26"/>
+      <c r="K30" s="31">
         <v>7.4778409999999997</v>
       </c>
-      <c r="L30" s="30">
+      <c r="L30" s="31">
         <v>7.4778409999999997</v>
       </c>
+      <c r="M30" s="32"/>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="66">
+        <v>88</v>
+      </c>
+      <c r="E31" s="65">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2889,9 +2987,9 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E32" s="66">
+        <v>89</v>
+      </c>
+      <c r="E32" s="65">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2907,9 +3005,9 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="66">
+        <v>90</v>
+      </c>
+      <c r="E33" s="65">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2925,9 +3023,9 @@
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="66">
+        <v>65</v>
+      </c>
+      <c r="E34" s="65">
         <f t="shared" si="5"/>
         <v>7.4851209999999995</v>
       </c>
@@ -2946,13 +3044,13 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="66">
+        <v>69</v>
+      </c>
+      <c r="E35" s="65">
         <f t="shared" si="5"/>
         <v>15.094021</v>
       </c>
-      <c r="F35" s="55">
+      <c r="F35" s="54">
         <v>4.2845839999999997</v>
       </c>
       <c r="K35" s="30">
@@ -2967,11 +3065,11 @@
         <v>5</v>
       </c>
       <c r="C36" s="26"/>
-      <c r="E36" s="67">
+      <c r="E36" s="66">
         <f>L36</f>
         <v>6.7462200000000001</v>
       </c>
-      <c r="F36" s="65">
+      <c r="F36" s="64">
         <v>3.6719759999999999</v>
       </c>
       <c r="G36" s="26"/>
@@ -2985,9 +3083,9 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E37" s="66">
+        <v>66</v>
+      </c>
+      <c r="E37" s="65">
         <f t="shared" si="5"/>
         <v>29.325361999999998</v>
       </c>
@@ -3006,9 +3104,9 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="66">
+        <v>67</v>
+      </c>
+      <c r="E39" s="65">
         <f t="shared" si="5"/>
         <v>4.1799999999999997E-3</v>
       </c>
@@ -3024,9 +3122,9 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="66">
+        <v>68</v>
+      </c>
+      <c r="E40" s="65">
         <f t="shared" si="5"/>
         <v>4.1799999999999997E-3</v>
       </c>
@@ -3045,9 +3143,9 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" s="66">
+        <v>70</v>
+      </c>
+      <c r="E41" s="65">
         <f t="shared" si="5"/>
         <v>0.12937000000000001</v>
       </c>
@@ -3063,9 +3161,9 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="66">
+        <v>67</v>
+      </c>
+      <c r="E42" s="65">
         <f t="shared" si="5"/>
         <v>3.2980000000000002E-3</v>
       </c>
@@ -3081,9 +3179,9 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E43" s="66">
+        <v>71</v>
+      </c>
+      <c r="E43" s="65">
         <f t="shared" si="5"/>
         <v>0.136848</v>
       </c>
@@ -3105,9 +3203,9 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="66">
+        <v>72</v>
+      </c>
+      <c r="E45" s="65">
         <f t="shared" si="5"/>
         <v>29.188514000000001</v>
       </c>
@@ -3123,9 +3221,9 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="66">
+        <v>73</v>
+      </c>
+      <c r="E46" s="65">
         <f t="shared" si="5"/>
         <v>29.325362000000002</v>
       </c>
@@ -3144,30 +3242,30 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E48" s="66">
+        <v>79</v>
+      </c>
+      <c r="E48" s="65">
         <f t="shared" si="5"/>
         <v>29.188513999999998</v>
       </c>
-      <c r="F48" s="55">
+      <c r="F48" s="54">
         <f>F37-F43</f>
         <v>5.2885609999999996</v>
       </c>
-      <c r="K48" s="55">
+      <c r="K48" s="54">
         <f>K37-K43</f>
         <v>19.895889999999998</v>
       </c>
-      <c r="L48" s="55">
+      <c r="L48" s="54">
         <f>L37-L43</f>
         <v>29.188513999999998</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E49" s="66">
+        <v>91</v>
+      </c>
+      <c r="E49" s="65">
         <f t="shared" si="5"/>
         <v>5.618491802492824E-2</v>
       </c>
@@ -3184,49 +3282,49 @@
         <v>5.618491802492824E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="68" customFormat="1">
-      <c r="A51" s="68" t="s">
+    <row r="51" spans="1:13" s="67" customFormat="1">
+      <c r="A51" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="E51" s="72">
+      <c r="C51" s="68"/>
+      <c r="E51" s="71">
         <f>E36+E30</f>
         <v>14.224060999999999</v>
       </c>
-      <c r="F51" s="71">
+      <c r="F51" s="70">
         <f>F36+F30</f>
         <v>3.6719759999999999</v>
       </c>
-      <c r="G51" s="69"/>
-      <c r="K51" s="71">
+      <c r="G51" s="68"/>
+      <c r="K51" s="70">
         <f t="shared" ref="K51:L51" si="8">K36+K30</f>
         <v>9.7642759999999988</v>
       </c>
-      <c r="L51" s="71">
+      <c r="L51" s="70">
         <f t="shared" si="8"/>
         <v>14.224060999999999</v>
       </c>
-      <c r="M51" s="70"/>
-    </row>
-    <row r="52" spans="1:13" s="68" customFormat="1">
-      <c r="A52" s="68" t="s">
+      <c r="M51" s="69"/>
+    </row>
+    <row r="52" spans="1:13" s="67" customFormat="1">
+      <c r="A52" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="69"/>
-      <c r="E52" s="69">
+      <c r="C52" s="68"/>
+      <c r="E52" s="68">
         <v>0</v>
       </c>
-      <c r="F52" s="68">
+      <c r="F52" s="67">
         <v>0</v>
       </c>
-      <c r="G52" s="69"/>
-      <c r="K52" s="68">
+      <c r="G52" s="68"/>
+      <c r="K52" s="67">
         <v>0</v>
       </c>
-      <c r="L52" s="68">
+      <c r="L52" s="67">
         <v>0</v>
       </c>
-      <c r="M52" s="70"/>
+      <c r="M52" s="69"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="2" t="s">
@@ -3236,15 +3334,15 @@
         <f>E51-E52</f>
         <v>14.224060999999999</v>
       </c>
-      <c r="F53" s="55">
+      <c r="F53" s="54">
         <f>F51-F52</f>
         <v>3.6719759999999999</v>
       </c>
-      <c r="K53" s="55">
+      <c r="K53" s="54">
         <f t="shared" ref="K53:L53" si="9">K51-K52</f>
         <v>9.7642759999999988</v>
       </c>
-      <c r="L53" s="55">
+      <c r="L53" s="54">
         <f t="shared" si="9"/>
         <v>14.224060999999999</v>
       </c>
@@ -3266,7 +3364,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
£BIDS new CFO news
</commit_message>
<xml_diff>
--- a/£BIDS.xlsx
+++ b/£BIDS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845E7AD-8A01-409A-87BA-E06B782D147F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E0CBEA-AED0-4FDA-A543-E781A7E33427}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="18900" activeTab="1" xr2:uid="{DFFD8AD2-463C-4EE9-AB45-D04A4DE50CB4}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29040" windowHeight="18900" xr2:uid="{DFFD8AD2-463C-4EE9-AB45-D04A4DE50CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
   <si>
     <t>£BIDS</t>
   </si>
@@ -380,6 +380,12 @@
   </si>
   <si>
     <t>Train Sim World 2/3</t>
+  </si>
+  <si>
+    <t>New CFO Thomas Bullen is appointed, shares rally +10% on this news</t>
+  </si>
+  <si>
+    <t>Thomas Bullen</t>
   </si>
 </sst>
 </file>
@@ -737,45 +743,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -788,6 +755,45 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1278,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCA1B8B-B033-42AF-8B6E-08E2900A293A}">
   <dimension ref="B2:AA43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1298,41 +1304,41 @@
       </c>
     </row>
     <row r="5" spans="2:27">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="83"/>
-      <c r="H5" s="81" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="H5" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="83"/>
-      <c r="S5" s="81" t="s">
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="84"/>
+      <c r="S5" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="83"/>
-      <c r="X5" s="81" t="s">
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="84"/>
+      <c r="X5" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="82"/>
-      <c r="AA5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="84"/>
     </row>
     <row r="6" spans="2:27">
       <c r="B6" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="31">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="D6" s="53"/>
       <c r="H6" s="37"/>
@@ -1344,12 +1350,12 @@
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
       <c r="P6" s="34"/>
-      <c r="S6" s="80" t="s">
+      <c r="S6" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="76"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="81"/>
       <c r="X6" s="35" t="s">
         <v>33</v>
       </c>
@@ -1367,8 +1373,12 @@
       <c r="D7" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="33"/>
+      <c r="H7" s="32">
+        <v>44958</v>
+      </c>
+      <c r="I7" s="70" t="s">
+        <v>118</v>
+      </c>
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
       <c r="L7" s="33"/>
@@ -1376,12 +1386,12 @@
       <c r="N7" s="33"/>
       <c r="O7" s="33"/>
       <c r="P7" s="34"/>
-      <c r="S7" s="80" t="s">
+      <c r="S7" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="75"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="76"/>
+      <c r="T7" s="80"/>
+      <c r="U7" s="80"/>
+      <c r="V7" s="81"/>
       <c r="X7" s="38" t="s">
         <v>117</v>
       </c>
@@ -1395,7 +1405,7 @@
       </c>
       <c r="C8" s="39">
         <f>C6*C7</f>
-        <v>26.11084</v>
+        <v>16.785539999999997</v>
       </c>
       <c r="D8" s="53"/>
       <c r="H8" s="37"/>
@@ -1407,12 +1417,12 @@
       <c r="N8" s="33"/>
       <c r="O8" s="33"/>
       <c r="P8" s="34"/>
-      <c r="S8" s="80" t="s">
+      <c r="S8" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="T8" s="75"/>
-      <c r="U8" s="75"/>
-      <c r="V8" s="76"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="80"/>
+      <c r="V8" s="81"/>
       <c r="X8" s="40"/>
       <c r="Y8" s="33"/>
       <c r="Z8" s="33"/>
@@ -1441,12 +1451,12 @@
       <c r="N9" s="33"/>
       <c r="O9" s="33"/>
       <c r="P9" s="34"/>
-      <c r="S9" s="80" t="s">
+      <c r="S9" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="76"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="81"/>
       <c r="X9" s="35" t="s">
         <v>34</v>
       </c>
@@ -1475,12 +1485,12 @@
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
-      <c r="S10" s="80" t="s">
+      <c r="S10" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75"/>
-      <c r="V10" s="76"/>
+      <c r="T10" s="80"/>
+      <c r="U10" s="80"/>
+      <c r="V10" s="81"/>
       <c r="X10" s="38" t="s">
         <v>42</v>
       </c>
@@ -1508,12 +1518,12 @@
       <c r="N11" s="33"/>
       <c r="O11" s="33"/>
       <c r="P11" s="34"/>
-      <c r="S11" s="80" t="s">
+      <c r="S11" s="85" t="s">
         <v>107</v>
       </c>
-      <c r="T11" s="75"/>
-      <c r="U11" s="75"/>
-      <c r="V11" s="76"/>
+      <c r="T11" s="80"/>
+      <c r="U11" s="80"/>
+      <c r="V11" s="81"/>
       <c r="X11" s="35"/>
       <c r="Y11" s="33"/>
       <c r="Z11" s="33"/>
@@ -1525,7 +1535,7 @@
       </c>
       <c r="C12" s="42">
         <f>C8-C11</f>
-        <v>22.41084</v>
+        <v>13.085539999999998</v>
       </c>
       <c r="D12" s="54"/>
       <c r="H12" s="37"/>
@@ -1537,12 +1547,12 @@
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
       <c r="P12" s="34"/>
-      <c r="S12" s="80" t="s">
+      <c r="S12" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="T12" s="75"/>
-      <c r="U12" s="75"/>
-      <c r="V12" s="76"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
+      <c r="V12" s="81"/>
       <c r="X12" s="35" t="s">
         <v>41</v>
       </c>
@@ -1567,12 +1577,12 @@
       <c r="N13" s="33"/>
       <c r="O13" s="33"/>
       <c r="P13" s="34"/>
-      <c r="S13" s="80" t="s">
+      <c r="S13" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="T13" s="75"/>
-      <c r="U13" s="75"/>
-      <c r="V13" s="76"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="80"/>
+      <c r="V13" s="81"/>
       <c r="X13" s="38" t="s">
         <v>61</v>
       </c>
@@ -1593,12 +1603,12 @@
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
-      <c r="S14" s="80" t="s">
+      <c r="S14" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="T14" s="75"/>
-      <c r="U14" s="75"/>
-      <c r="V14" s="76"/>
+      <c r="T14" s="80"/>
+      <c r="U14" s="80"/>
+      <c r="V14" s="81"/>
       <c r="X14" s="38" t="s">
         <v>75</v>
       </c>
@@ -1607,11 +1617,11 @@
       <c r="AA14" s="34"/>
     </row>
     <row r="15" spans="2:27">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="84"/>
       <c r="H15" s="37"/>
       <c r="I15" s="33"/>
       <c r="J15" s="33"/>
@@ -1621,12 +1631,12 @@
       <c r="N15" s="33"/>
       <c r="O15" s="33"/>
       <c r="P15" s="34"/>
-      <c r="S15" s="80" t="s">
+      <c r="S15" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="T15" s="75"/>
-      <c r="U15" s="75"/>
-      <c r="V15" s="76"/>
+      <c r="T15" s="80"/>
+      <c r="U15" s="80"/>
+      <c r="V15" s="81"/>
       <c r="X15" s="40"/>
       <c r="Y15" s="33"/>
       <c r="Z15" s="33"/>
@@ -1636,10 +1646,10 @@
       <c r="B16" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="81"/>
       <c r="H16" s="37"/>
       <c r="I16" s="33"/>
       <c r="J16" s="33"/>
@@ -1649,12 +1659,12 @@
       <c r="N16" s="33"/>
       <c r="O16" s="33"/>
       <c r="P16" s="34"/>
-      <c r="S16" s="77" t="s">
+      <c r="S16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="T16" s="78"/>
-      <c r="U16" s="78"/>
-      <c r="V16" s="79"/>
+      <c r="T16" s="86"/>
+      <c r="U16" s="86"/>
+      <c r="V16" s="87"/>
       <c r="X16" s="35" t="s">
         <v>35</v>
       </c>
@@ -1666,8 +1676,10 @@
       <c r="B17" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="76"/>
+      <c r="C17" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="81"/>
       <c r="H17" s="32">
         <v>44743</v>
       </c>
@@ -1692,10 +1704,10 @@
       <c r="B18" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="76"/>
+      <c r="D18" s="81"/>
       <c r="H18" s="37"/>
       <c r="I18" s="50" t="s">
         <v>78</v>
@@ -1716,10 +1728,10 @@
       <c r="B19" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="80" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="76"/>
+      <c r="D19" s="81"/>
       <c r="H19" s="37"/>
       <c r="I19" s="33"/>
       <c r="J19" s="33"/>
@@ -1740,10 +1752,10 @@
       <c r="B20" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="79"/>
+      <c r="D20" s="87"/>
       <c r="H20" s="37"/>
       <c r="I20" s="33"/>
       <c r="J20" s="33"/>
@@ -1791,11 +1803,11 @@
       <c r="AA22" s="34"/>
     </row>
     <row r="23" spans="2:27">
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="82"/>
-      <c r="D23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="84"/>
       <c r="H23" s="37"/>
       <c r="I23" s="33"/>
       <c r="J23" s="33"/>
@@ -1816,10 +1828,10 @@
       <c r="B24" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="76"/>
+      <c r="D24" s="81"/>
       <c r="H24" s="37"/>
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
@@ -1840,10 +1852,10 @@
       <c r="B25" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="75">
+      <c r="C25" s="80">
         <v>2016</v>
       </c>
-      <c r="D25" s="76"/>
+      <c r="D25" s="81"/>
       <c r="H25" s="37"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
@@ -1862,8 +1874,8 @@
     </row>
     <row r="26" spans="2:27">
       <c r="B26" s="37"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
       <c r="H26" s="37"/>
       <c r="I26" s="33"/>
       <c r="J26" s="33"/>
@@ -1896,13 +1908,13 @@
     </row>
     <row r="28" spans="2:27">
       <c r="B28" s="37"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="76"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
     </row>
     <row r="29" spans="2:27">
       <c r="B29" s="37"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="76"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
     </row>
     <row r="30" spans="2:27">
       <c r="B30" s="37" t="s">
@@ -1917,27 +1929,27 @@
       <c r="B31" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="87"/>
+      <c r="D31" s="91"/>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="84"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="84">
+      <c r="C35" s="88">
         <f>C8/'Financial Model'!C14+'Financial Model'!C14</f>
-        <v>-11.241799745553379</v>
-      </c>
-      <c r="D35" s="85"/>
+        <v>-8.3980051935700288</v>
+      </c>
+      <c r="D35" s="89"/>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="37" t="s">
@@ -1950,8 +1962,8 @@
       <c r="B37" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="76"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="81"/>
       <c r="H37" s="2" t="s">
         <v>103</v>
       </c>
@@ -1960,62 +1972,52 @@
       <c r="B38" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="76"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="81"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="84">
+      <c r="C39" s="88">
         <f>C6/'Financial Model'!F49</f>
-        <v>4.9319434991862634</v>
-      </c>
-      <c r="D39" s="85"/>
+        <v>3.1705351066197403</v>
+      </c>
+      <c r="D39" s="89"/>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="37"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="76"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="81"/>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="75"/>
-      <c r="D41" s="76"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81"/>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C42" s="75"/>
-      <c r="D42" s="76"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="78"/>
-      <c r="D43" s="79"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="H5:P5"/>
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="S5:V5"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="S7:V7"/>
-    <mergeCell ref="S8:V8"/>
+    <mergeCell ref="S16:V16"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="S13:V13"/>
+    <mergeCell ref="S14:V14"/>
+    <mergeCell ref="S15:V15"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
@@ -2032,20 +2034,31 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="H5:P5"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="S10:V10"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="S7:V7"/>
+    <mergeCell ref="S8:V8"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="S16:V16"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="S13:V13"/>
-    <mergeCell ref="S14:V14"/>
-    <mergeCell ref="S15:V15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{E4B851AE-A6B7-0248-9880-6DBD666C28BA}"/>
     <hyperlink ref="I9" r:id="rId2" display="Bidstack appoint Camila Franklin as COO" xr:uid="{91406AA9-3DB6-4F3F-9F60-8807BC447FC0}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{BFCBC1AD-F0CC-4B55-895C-A3C604C10E16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2053,11 +2066,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E293192-11D7-45EA-B129-F04B731A5D6C}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2108,43 +2121,43 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="88" customFormat="1">
+    <row r="2" spans="1:20" s="75" customFormat="1">
       <c r="A2" s="6"/>
-      <c r="B2" s="89">
+      <c r="B2" s="76">
         <v>44012</v>
       </c>
-      <c r="C2" s="90">
+      <c r="C2" s="77">
         <v>44196</v>
       </c>
-      <c r="D2" s="89">
+      <c r="D2" s="76">
         <v>44377</v>
       </c>
-      <c r="E2" s="90">
+      <c r="E2" s="77">
         <v>44561</v>
       </c>
-      <c r="F2" s="89">
+      <c r="F2" s="76">
         <v>44742</v>
       </c>
-      <c r="G2" s="90"/>
-      <c r="J2" s="89">
+      <c r="G2" s="77"/>
+      <c r="J2" s="76">
         <v>43830</v>
       </c>
-      <c r="K2" s="89">
+      <c r="K2" s="76">
         <v>44196</v>
       </c>
-      <c r="L2" s="89">
+      <c r="L2" s="76">
         <v>44561</v>
       </c>
-      <c r="M2" s="91" t="s">
+      <c r="M2" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="6" t="s">

</xml_diff>